<commit_message>
UST Fair mp3 and glossary virtual cursor
</commit_message>
<xml_diff>
--- a/public/assets/askFuture/glossary.xlsx
+++ b/public/assets/askFuture/glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\新增資料夾\askFuture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\FUTURE Promotion Event\20230513_HKUST School of Engineering Exploration Day\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1915F523-06FD-4482-9B1B-74A3134D6EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B87FCC3E-78B8-47AC-9E25-CEDD000436A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{57FFC4F2-4720-43F9-9096-B2F8DDB185DB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="215">
   <si>
     <t>Image Name</t>
   </si>
@@ -626,6 +626,60 @@
   </si>
   <si>
     <t>Cookie.m4a</t>
+  </si>
+  <si>
+    <t>Future 1.jpg</t>
+  </si>
+  <si>
+    <t>Future 2.jpg</t>
+  </si>
+  <si>
+    <t>Future 3.jpg</t>
+  </si>
+  <si>
+    <t>Future 5.jpg</t>
+  </si>
+  <si>
+    <t>Future 4.jpg</t>
+  </si>
+  <si>
+    <t>Future 6.jpg</t>
+  </si>
+  <si>
+    <t>Section1 Welcome.mp3</t>
+  </si>
+  <si>
+    <t>Section2 Always.mp3</t>
+  </si>
+  <si>
+    <t>Section3 Journey.mp3</t>
+  </si>
+  <si>
+    <t>Section4 Anything.mp3</t>
+  </si>
+  <si>
+    <t>Section5 Engineering.mp3</t>
+  </si>
+  <si>
+    <t>Section6 Have.mp3</t>
+  </si>
+  <si>
+    <t>/good day/,/bye/</t>
+  </si>
+  <si>
+    <t>/journey/,/destination/</t>
+  </si>
+  <si>
+    <t>/curious/,/embrace/,/</t>
+  </si>
+  <si>
+    <t>/welcome/,/nervous/,/interview/</t>
+  </si>
+  <si>
+    <t>/anything/,/design/</t>
+  </si>
+  <si>
+    <t>/engineering/</t>
   </si>
 </sst>
 </file>
@@ -977,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3960D156-2B6A-42FF-9B6C-1CAC0FD4699A}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,6 +2087,108 @@
         <v>196</v>
       </c>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" t="s">
+        <v>212</v>
+      </c>
+      <c r="D62" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" t="s">
+        <v>211</v>
+      </c>
+      <c r="D63" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>115</v>
+      </c>
+      <c r="B65" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" t="s">
+        <v>213</v>
+      </c>
+      <c r="D65" t="s">
+        <v>201</v>
+      </c>
+      <c r="E65" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" t="s">
+        <v>200</v>
+      </c>
+      <c r="E66" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" t="s">
+        <v>115</v>
+      </c>
+      <c r="C67" t="s">
+        <v>209</v>
+      </c>
+      <c r="D67" t="s">
+        <v>202</v>
+      </c>
+      <c r="E67" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>